<commit_message>
update hainan aqua chart1
</commit_message>
<xml_diff>
--- a/src/main/resources/data/hainan/水产养殖.xlsx
+++ b/src/main/resources/data/hainan/水产养殖.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="791" firstSheet="2" activeTab="2"/>
+    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="791"/>
   </bookViews>
   <sheets>
-    <sheet name="左1-近年海水养殖面积情况" sheetId="2" r:id="rId1"/>
+    <sheet name="左1-近年水产品养殖面积及构成" sheetId="2" r:id="rId1"/>
     <sheet name="左2-近年淡水养殖面积情况" sheetId="4" r:id="rId2"/>
     <sheet name="左3 -近年海水养殖各类面积占比" sheetId="3" r:id="rId3"/>
     <sheet name="右1-近年水产品总产量情况" sheetId="12" r:id="rId4"/>
@@ -34,15 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+  <si>
+    <t>水产品养殖（万亩）</t>
+  </si>
+  <si>
+    <t>海水养殖(万亩)</t>
+  </si>
+  <si>
+    <t>淡水养殖(万亩)</t>
+  </si>
   <si>
     <t>水产养殖</t>
-  </si>
-  <si>
-    <t>海水养殖(万亩)</t>
-  </si>
-  <si>
-    <t>淡水养殖(万亩)</t>
   </si>
   <si>
     <t>鱼类</t>
@@ -155,14 +158,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="28">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -720,133 +716,133 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -860,50 +856,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1224,63 +1220,97 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="2" width="15.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:2">
-      <c r="A1" s="11" t="s">
+    <row r="1" ht="15.75" spans="1:4">
+      <c r="A1" s="11"/>
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:2">
+      <c r="D1" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="13">
         <v>2018</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="17">
+        <v>78.26</v>
+      </c>
+      <c r="C2" s="17">
         <v>32.058</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" spans="1:2">
+      <c r="D2" s="17">
+        <v>46.2</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:4">
       <c r="A3" s="13">
         <v>2019</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="17">
+        <v>76.95</v>
+      </c>
+      <c r="C3" s="17">
         <v>30.765</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" spans="1:2">
+      <c r="D3" s="17">
+        <v>46.188</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="13">
         <v>2020</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="17">
+        <v>66.9</v>
+      </c>
+      <c r="C4" s="17">
         <v>26.394</v>
       </c>
-    </row>
-    <row r="5" ht="15.75" spans="1:2">
+      <c r="D4" s="17">
+        <v>40.5075</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="13">
         <v>2021</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="17">
+        <v>67.51</v>
+      </c>
+      <c r="C5" s="17">
         <v>23.8215</v>
       </c>
-    </row>
-    <row r="6" ht="15.75" spans="1:2">
+      <c r="D5" s="17">
+        <v>43.6875</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="13">
         <v>2022</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="17">
+        <v>67.44</v>
+      </c>
+      <c r="C6" s="17">
         <v>23.391</v>
+      </c>
+      <c r="D6" s="17">
+        <v>44.046</v>
       </c>
     </row>
     <row r="7" ht="15"/>
@@ -1307,36 +1337,36 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:8">
       <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" ht="15.75" spans="1:8">
       <c r="A2" s="13">
         <v>2018</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="10">
         <v>46.2</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" ht="15.75" spans="1:8">
       <c r="A3" s="13">
         <v>2019</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="10">
         <v>46.188</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" ht="15.75" spans="1:2">
       <c r="A4" s="13">
         <v>2020</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="10">
         <v>40.5075</v>
       </c>
     </row>
@@ -1344,7 +1374,7 @@
       <c r="A5" s="13">
         <v>2021</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="10">
         <v>43.6875</v>
       </c>
     </row>
@@ -1352,17 +1382,17 @@
       <c r="A6" s="13">
         <v>2022</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="10">
         <v>44.046</v>
       </c>
     </row>
     <row r="7" ht="15"/>
     <row r="9" spans="8:12">
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1375,7 +1405,7 @@
   <sheetPr/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -1387,47 +1417,47 @@
   <sheetData>
     <row r="1" ht="48.75" customHeight="1" spans="1:2">
       <c r="A1" s="11"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
       <c r="A2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="16">
+        <v>4</v>
+      </c>
+      <c r="B2" s="10">
         <v>8.1975</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:2">
       <c r="A3" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="16">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10">
         <v>11.871</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:2">
       <c r="A4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="16">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10">
         <v>3.03</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:2">
       <c r="A5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="16">
+        <v>7</v>
+      </c>
+      <c r="B5" s="10">
         <v>0.129</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" ht="15.75" spans="1:2">
       <c r="A6" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="16">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10">
         <v>0.162</v>
       </c>
     </row>
@@ -1455,17 +1485,17 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
       <c r="A2" s="13">
         <v>2018</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="10">
         <v>175.8188</v>
       </c>
     </row>
@@ -1473,7 +1503,7 @@
       <c r="A3" s="13">
         <v>2019</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="10">
         <v>172.1571</v>
       </c>
     </row>
@@ -1481,7 +1511,7 @@
       <c r="A4" s="13">
         <v>2020</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="10">
         <v>166.7878</v>
       </c>
     </row>
@@ -1489,7 +1519,7 @@
       <c r="A5" s="13">
         <v>2021</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="10">
         <v>164.0918</v>
       </c>
     </row>
@@ -1497,7 +1527,7 @@
       <c r="A6" s="13">
         <v>2022</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="10">
         <v>170.311</v>
       </c>
     </row>
@@ -1524,13 +1554,13 @@
   <sheetData>
     <row r="1" ht="58.5" spans="1:3">
       <c r="A1" s="11" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:3">
@@ -1611,10 +1641,10 @@
   <sheetData>
     <row r="1" ht="58.5" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
@@ -1680,15 +1710,15 @@
   <sheetData>
     <row r="1" ht="44.25" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
       <c r="A2" s="13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="14">
         <v>135.0215</v>
@@ -1696,7 +1726,7 @@
     </row>
     <row r="3" ht="15.75" spans="1:2">
       <c r="A3" s="13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="14">
         <v>18.0277</v>
@@ -1704,7 +1734,7 @@
     </row>
     <row r="4" ht="15.75" spans="1:2">
       <c r="A4" s="13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="14">
         <v>4.6479</v>
@@ -1712,7 +1742,7 @@
     </row>
     <row r="5" ht="15.75" spans="1:2">
       <c r="A5" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="14">
         <v>1.0929</v>
@@ -1720,7 +1750,7 @@
     </row>
     <row r="6" ht="15.75" spans="1:2">
       <c r="A6" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="14">
         <v>11.521</v>
@@ -1753,24 +1783,24 @@
   <sheetData>
     <row r="1" ht="15" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" ht="15" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="6">
         <v>3.6735</v>
@@ -1787,7 +1817,7 @@
     </row>
     <row r="3" ht="15" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6">
         <v>0.144</v>
@@ -1804,7 +1834,7 @@
     </row>
     <row r="4" ht="15" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="6">
         <v>3.909</v>
@@ -1821,7 +1851,7 @@
     </row>
     <row r="5" ht="15" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="6">
         <v>0.7935</v>
@@ -1838,7 +1868,7 @@
     </row>
     <row r="6" ht="15" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6">
         <v>6.228</v>
@@ -1855,7 +1885,7 @@
     </row>
     <row r="7" ht="15" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6">
         <v>1.3905</v>
@@ -1872,7 +1902,7 @@
     </row>
     <row r="8" ht="15" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6">
         <v>0.75</v>
@@ -1889,7 +1919,7 @@
     </row>
     <row r="9" ht="15" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -1902,7 +1932,7 @@
     </row>
     <row r="10" ht="15" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="6">
         <v>0.9195</v>
@@ -1919,7 +1949,7 @@
     </row>
     <row r="11" ht="15" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="6">
         <v>2.0025</v>
@@ -1936,7 +1966,7 @@
     </row>
     <row r="12" ht="15" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="6">
         <v>2.013</v>
@@ -1953,7 +1983,7 @@
     </row>
     <row r="13" ht="15" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6">
@@ -1966,7 +1996,7 @@
     </row>
     <row r="14" ht="15" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6">
@@ -1979,7 +2009,7 @@
     </row>
     <row r="15" ht="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="6">
         <v>1.008</v>
@@ -1996,7 +2026,7 @@
     </row>
     <row r="16" ht="15" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="6">
         <v>0.5595</v>
@@ -2013,7 +2043,7 @@
     </row>
     <row r="17" ht="15" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6">
@@ -2026,7 +2056,7 @@
     </row>
     <row r="18" ht="15" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -2039,7 +2069,7 @@
     </row>
     <row r="19" ht="15" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6">

</xml_diff>

<commit_message>
update hainan aqua chart2
</commit_message>
<xml_diff>
--- a/src/main/resources/data/hainan/水产养殖.xlsx
+++ b/src/main/resources/data/hainan/水产养殖.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="791"/>
+    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="791" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="左1-近年水产品养殖面积及构成" sheetId="2" r:id="rId1"/>
-    <sheet name="左2-近年淡水养殖面积情况" sheetId="4" r:id="rId2"/>
+    <sheet name="左2-近年水产品产量及构成" sheetId="4" r:id="rId2"/>
     <sheet name="左3 -近年海水养殖各类面积占比" sheetId="3" r:id="rId3"/>
     <sheet name="右1-近年水产品总产量情况" sheetId="12" r:id="rId4"/>
     <sheet name="右2-近年海水产品产量情况" sheetId="13" r:id="rId5"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>水产品养殖（万亩）</t>
   </si>
@@ -45,22 +45,33 @@
     <t>淡水养殖(万亩)</t>
   </si>
   <si>
+    <t>总产量(万吨)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">海水产品万吨)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">淡水产品(万吨)
+</t>
+  </si>
+  <si>
+    <t>鱼类</t>
+  </si>
+  <si>
+    <t>虾蟹类</t>
+  </si>
+  <si>
+    <t>贝类</t>
+  </si>
+  <si>
+    <t>藻类</t>
+  </si>
+  <si>
+    <t>其他</t>
+  </si>
+  <si>
     <t>水产养殖</t>
-  </si>
-  <si>
-    <t>鱼类</t>
-  </si>
-  <si>
-    <t>虾蟹类</t>
-  </si>
-  <si>
-    <t>贝类</t>
-  </si>
-  <si>
-    <t>藻类</t>
-  </si>
-  <si>
-    <t>其他</t>
   </si>
   <si>
     <t>水产品总产量(万吨)</t>
@@ -158,7 +169,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,13 +212,6 @@
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -716,137 +720,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -897,9 +901,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1222,7 +1223,7 @@
   <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
@@ -1233,13 +1234,13 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="11"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1247,13 +1248,13 @@
       <c r="A2" s="13">
         <v>2018</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="10">
         <v>78.26</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="10">
         <v>32.058</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="10">
         <v>46.2</v>
       </c>
     </row>
@@ -1261,13 +1262,13 @@
       <c r="A3" s="13">
         <v>2019</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="10">
         <v>76.95</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="10">
         <v>30.765</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="10">
         <v>46.188</v>
       </c>
     </row>
@@ -1275,13 +1276,13 @@
       <c r="A4" s="13">
         <v>2020</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="10">
         <v>66.9</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="10">
         <v>26.394</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="10">
         <v>40.5075</v>
       </c>
     </row>
@@ -1289,13 +1290,13 @@
       <c r="A5" s="13">
         <v>2021</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="10">
         <v>67.51</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="10">
         <v>23.8215</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="10">
         <v>43.6875</v>
       </c>
     </row>
@@ -1303,13 +1304,13 @@
       <c r="A6" s="13">
         <v>2022</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="10">
         <v>67.44</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="10">
         <v>23.391</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="10">
         <v>44.046</v>
       </c>
     </row>
@@ -1326,8 +1327,8 @@
   <sheetPr/>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1335,12 +1336,16 @@
     <col min="2" max="2" width="12.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:8">
-      <c r="A1" s="11" t="s">
+    <row r="1" ht="39.75" spans="1:8">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>2</v>
+      <c r="C1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="H1" s="16"/>
     </row>
@@ -1348,8 +1353,14 @@
       <c r="A2" s="13">
         <v>2018</v>
       </c>
-      <c r="B2" s="10">
-        <v>46.2</v>
+      <c r="B2" s="13">
+        <v>175.8188</v>
+      </c>
+      <c r="C2" s="13">
+        <v>137.8071</v>
+      </c>
+      <c r="D2" s="13">
+        <v>38.0117</v>
       </c>
       <c r="H2" s="16"/>
     </row>
@@ -1357,33 +1368,57 @@
       <c r="A3" s="13">
         <v>2019</v>
       </c>
-      <c r="B3" s="10">
-        <v>46.188</v>
+      <c r="B3" s="13">
+        <v>172.1571</v>
+      </c>
+      <c r="C3" s="13">
+        <v>135.0103</v>
+      </c>
+      <c r="D3" s="13">
+        <v>37.1468</v>
       </c>
       <c r="H3" s="16"/>
     </row>
-    <row r="4" ht="15.75" spans="1:2">
+    <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="13">
         <v>2020</v>
       </c>
-      <c r="B4" s="10">
-        <v>40.5075</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" spans="1:2">
+      <c r="B4" s="13">
+        <v>166.7878</v>
+      </c>
+      <c r="C4" s="13">
+        <v>130.2591</v>
+      </c>
+      <c r="D4" s="13">
+        <v>36.5287</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="13">
         <v>2021</v>
       </c>
-      <c r="B5" s="10">
-        <v>43.6875</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" spans="1:2">
+      <c r="B5" s="13">
+        <v>164.0918</v>
+      </c>
+      <c r="C5" s="13">
+        <v>127.3762</v>
+      </c>
+      <c r="D5" s="13">
+        <v>36.7156</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="13">
         <v>2022</v>
       </c>
-      <c r="B6" s="10">
-        <v>44.046</v>
+      <c r="B6" s="13">
+        <v>170.311</v>
+      </c>
+      <c r="C6" s="13">
+        <v>128.0529</v>
+      </c>
+      <c r="D6" s="13">
+        <v>42.2581</v>
       </c>
     </row>
     <row r="7" ht="15"/>
@@ -1423,7 +1458,7 @@
     </row>
     <row r="2" ht="15.75" spans="1:2">
       <c r="A2" s="13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="10">
         <v>8.1975</v>
@@ -1431,7 +1466,7 @@
     </row>
     <row r="3" ht="15.75" spans="1:2">
       <c r="A3" s="13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="10">
         <v>11.871</v>
@@ -1439,7 +1474,7 @@
     </row>
     <row r="4" ht="15.75" spans="1:2">
       <c r="A4" s="13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="10">
         <v>3.03</v>
@@ -1447,7 +1482,7 @@
     </row>
     <row r="5" ht="15.75" spans="1:2">
       <c r="A5" s="13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="10">
         <v>0.129</v>
@@ -1455,7 +1490,7 @@
     </row>
     <row r="6" ht="15.75" spans="1:2">
       <c r="A6" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="10">
         <v>0.162</v>
@@ -1485,10 +1520,10 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
@@ -1554,13 +1589,13 @@
   <sheetData>
     <row r="1" ht="58.5" spans="1:3">
       <c r="A1" s="11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:3">
@@ -1641,10 +1676,10 @@
   <sheetData>
     <row r="1" ht="58.5" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
@@ -1710,15 +1745,15 @@
   <sheetData>
     <row r="1" ht="44.25" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
       <c r="A2" s="13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="14">
         <v>135.0215</v>
@@ -1726,7 +1761,7 @@
     </row>
     <row r="3" ht="15.75" spans="1:2">
       <c r="A3" s="13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="14">
         <v>18.0277</v>
@@ -1734,7 +1769,7 @@
     </row>
     <row r="4" ht="15.75" spans="1:2">
       <c r="A4" s="13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="14">
         <v>4.6479</v>
@@ -1742,7 +1777,7 @@
     </row>
     <row r="5" ht="15.75" spans="1:2">
       <c r="A5" s="13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="14">
         <v>1.0929</v>
@@ -1750,7 +1785,7 @@
     </row>
     <row r="6" ht="15.75" spans="1:2">
       <c r="A6" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="14">
         <v>11.521</v>
@@ -1783,24 +1818,24 @@
   <sheetData>
     <row r="1" ht="15" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" ht="15" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="6">
         <v>3.6735</v>
@@ -1817,7 +1852,7 @@
     </row>
     <row r="3" ht="15" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3" s="6">
         <v>0.144</v>
@@ -1834,7 +1869,7 @@
     </row>
     <row r="4" ht="15" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" s="6">
         <v>3.909</v>
@@ -1851,7 +1886,7 @@
     </row>
     <row r="5" ht="15" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="6">
         <v>0.7935</v>
@@ -1868,7 +1903,7 @@
     </row>
     <row r="6" ht="15" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6" s="6">
         <v>6.228</v>
@@ -1885,7 +1920,7 @@
     </row>
     <row r="7" ht="15" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B7" s="6">
         <v>1.3905</v>
@@ -1902,7 +1937,7 @@
     </row>
     <row r="8" ht="15" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" s="6">
         <v>0.75</v>
@@ -1919,7 +1954,7 @@
     </row>
     <row r="9" ht="15" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -1932,7 +1967,7 @@
     </row>
     <row r="10" ht="15" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="6">
         <v>0.9195</v>
@@ -1949,7 +1984,7 @@
     </row>
     <row r="11" ht="15" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6">
         <v>2.0025</v>
@@ -1966,7 +2001,7 @@
     </row>
     <row r="12" ht="15" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B12" s="6">
         <v>2.013</v>
@@ -1983,7 +2018,7 @@
     </row>
     <row r="13" ht="15" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6">
@@ -1996,7 +2031,7 @@
     </row>
     <row r="14" ht="15" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6">
@@ -2009,7 +2044,7 @@
     </row>
     <row r="15" ht="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B15" s="6">
         <v>1.008</v>
@@ -2026,7 +2061,7 @@
     </row>
     <row r="16" ht="15" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B16" s="6">
         <v>0.5595</v>
@@ -2043,7 +2078,7 @@
     </row>
     <row r="17" ht="15" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6">
@@ -2056,7 +2091,7 @@
     </row>
     <row r="18" ht="15" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -2069,7 +2104,7 @@
     </row>
     <row r="19" ht="15" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6">

</xml_diff>

<commit_message>
update hainan aqua chart3
</commit_message>
<xml_diff>
--- a/src/main/resources/data/hainan/水产养殖.xlsx
+++ b/src/main/resources/data/hainan/水产养殖.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="791" activeTab="1"/>
+    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="791" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="左1-近年水产品养殖面积及构成" sheetId="2" r:id="rId1"/>
     <sheet name="左2-近年水产品产量及构成" sheetId="4" r:id="rId2"/>
     <sheet name="左3 -近年海水养殖各类面积占比" sheetId="3" r:id="rId3"/>
-    <sheet name="右1-近年水产品总产量情况" sheetId="12" r:id="rId4"/>
+    <sheet name="右1-近年养殖水产品产量及构成" sheetId="12" r:id="rId4"/>
     <sheet name="右2-近年海水产品产量情况" sheetId="13" r:id="rId5"/>
     <sheet name="右3-近年淡水产品产量情况" sheetId="14" r:id="rId6"/>
     <sheet name="中下--2022各品类产量情况" sheetId="11" r:id="rId7"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>水产品养殖（万亩）</t>
   </si>
@@ -71,10 +71,15 @@
     <t>其他</t>
   </si>
   <si>
+    <t xml:space="preserve">海水养殖（万吨)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">淡水养殖(万吨)
+</t>
+  </si>
+  <si>
     <t>水产养殖</t>
-  </si>
-  <si>
-    <t>水产品总产量(万吨)</t>
   </si>
   <si>
     <t xml:space="preserve">海水产品产量(万吨)
@@ -1327,7 +1332,7 @@
   <sheetPr/>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -1507,63 +1512,79 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="2" max="2" width="20.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:2">
-      <c r="A1" s="11" t="s">
+    <row r="1" ht="39.75" spans="1:3">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:2">
+    <row r="2" ht="15.75" spans="1:3">
       <c r="A2" s="13">
         <v>2018</v>
       </c>
-      <c r="B2" s="10">
-        <v>175.8188</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" spans="1:2">
+      <c r="B2" s="13">
+        <v>29.42</v>
+      </c>
+      <c r="C2" s="13">
+        <v>36.69</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="13">
         <v>2019</v>
       </c>
-      <c r="B3" s="10">
-        <v>172.1571</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" spans="1:2">
+      <c r="B3" s="13">
+        <v>27.1</v>
+      </c>
+      <c r="C3" s="13">
+        <v>35.44</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:3">
       <c r="A4" s="13">
         <v>2020</v>
       </c>
-      <c r="B4" s="10">
-        <v>166.7878</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" spans="1:2">
+      <c r="B4" s="13">
+        <v>26.65</v>
+      </c>
+      <c r="C4" s="13">
+        <v>35.09</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:3">
       <c r="A5" s="13">
         <v>2021</v>
       </c>
-      <c r="B5" s="10">
-        <v>164.0918</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" spans="1:2">
+      <c r="B5" s="13">
+        <v>27.3</v>
+      </c>
+      <c r="C5" s="13">
+        <v>35.18</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:3">
       <c r="A6" s="13">
         <v>2022</v>
       </c>
-      <c r="B6" s="10">
-        <v>170.311</v>
+      <c r="B6" s="13">
+        <v>26.26</v>
+      </c>
+      <c r="C6" s="13">
+        <v>41.08</v>
       </c>
     </row>
     <row r="7" ht="15"/>
@@ -1589,13 +1610,13 @@
   <sheetData>
     <row r="1" ht="58.5" spans="1:3">
       <c r="A1" s="11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:3">
@@ -1676,10 +1697,10 @@
   <sheetData>
     <row r="1" ht="58.5" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
@@ -1745,10 +1766,10 @@
   <sheetData>
     <row r="1" ht="44.25" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
@@ -1818,24 +1839,24 @@
   <sheetData>
     <row r="1" ht="15" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" ht="15" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="6">
         <v>3.6735</v>
@@ -1852,7 +1873,7 @@
     </row>
     <row r="3" ht="15" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="6">
         <v>0.144</v>
@@ -1869,7 +1890,7 @@
     </row>
     <row r="4" ht="15" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="6">
         <v>3.909</v>
@@ -1886,7 +1907,7 @@
     </row>
     <row r="5" ht="15" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="6">
         <v>0.7935</v>
@@ -1903,7 +1924,7 @@
     </row>
     <row r="6" ht="15" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="6">
         <v>6.228</v>
@@ -1920,7 +1941,7 @@
     </row>
     <row r="7" ht="15" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="6">
         <v>1.3905</v>
@@ -1937,7 +1958,7 @@
     </row>
     <row r="8" ht="15" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="6">
         <v>0.75</v>
@@ -1954,7 +1975,7 @@
     </row>
     <row r="9" ht="15" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -1967,7 +1988,7 @@
     </row>
     <row r="10" ht="15" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="6">
         <v>0.9195</v>
@@ -1984,7 +2005,7 @@
     </row>
     <row r="11" ht="15" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="6">
         <v>2.0025</v>
@@ -2001,7 +2022,7 @@
     </row>
     <row r="12" ht="15" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="6">
         <v>2.013</v>
@@ -2018,7 +2039,7 @@
     </row>
     <row r="13" ht="15" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6">
@@ -2031,7 +2052,7 @@
     </row>
     <row r="14" ht="15" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6">
@@ -2044,7 +2065,7 @@
     </row>
     <row r="15" ht="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="6">
         <v>1.008</v>
@@ -2061,7 +2082,7 @@
     </row>
     <row r="16" ht="15" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" s="6">
         <v>0.5595</v>
@@ -2078,7 +2099,7 @@
     </row>
     <row r="17" ht="15" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6">
@@ -2091,7 +2112,7 @@
     </row>
     <row r="18" ht="15" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -2104,7 +2125,7 @@
     </row>
     <row r="19" ht="15" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6">

</xml_diff>

<commit_message>
update hainan aqua chart_6
</commit_message>
<xml_diff>
--- a/src/main/resources/data/hainan/水产养殖.xlsx
+++ b/src/main/resources/data/hainan/水产养殖.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="791" activeTab="3"/>
+    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="791" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="左1-近年水产品养殖面积及构成" sheetId="2" r:id="rId1"/>
     <sheet name="左2-近年水产品产量及构成" sheetId="4" r:id="rId2"/>
     <sheet name="左3 -近年海水养殖各类面积占比" sheetId="3" r:id="rId3"/>
     <sheet name="右1-近年养殖水产品产量及构成" sheetId="12" r:id="rId4"/>
-    <sheet name="右2-近年海水产品产量情况" sheetId="13" r:id="rId5"/>
+    <sheet name="右2-近年捕捞水产品产量及构成" sheetId="13" r:id="rId5"/>
     <sheet name="右3-近年淡水产品产量情况" sheetId="14" r:id="rId6"/>
     <sheet name="中下--2022各品类产量情况" sheetId="11" r:id="rId7"/>
     <sheet name="地图-2022年各市县水产养殖情况（面积、产量）" sheetId="9" r:id="rId8"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>水产品养殖（万亩）</t>
   </si>
@@ -79,11 +79,15 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">海水捕捞（万吨)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">淡水捕捞（万吨)
+</t>
+  </si>
+  <si>
     <t>水产养殖</t>
-  </si>
-  <si>
-    <t xml:space="preserve">海水产品产量(万吨)
-</t>
   </si>
   <si>
     <t xml:space="preserve">淡水产品产量(万吨)
@@ -174,7 +178,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,12 +213,6 @@
     <font>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -725,137 +723,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -899,9 +897,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1352,7 +1347,7 @@
       <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" ht="15.75" spans="1:8">
       <c r="A2" s="13">
@@ -1367,7 +1362,7 @@
       <c r="D2" s="13">
         <v>38.0117</v>
       </c>
-      <c r="H2" s="16"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" ht="15.75" spans="1:8">
       <c r="A3" s="13">
@@ -1382,7 +1377,7 @@
       <c r="D3" s="13">
         <v>37.1468</v>
       </c>
-      <c r="H3" s="16"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="13">
@@ -1428,11 +1423,11 @@
     </row>
     <row r="7" ht="15"/>
     <row r="9" spans="8:12">
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1514,7 +1509,7 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1599,8 +1594,8 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -1608,14 +1603,12 @@
     <col min="2" max="3" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="58.5" spans="1:3">
-      <c r="A1" s="11" t="s">
+    <row r="1" ht="39.75" spans="1:3">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1623,55 +1616,55 @@
       <c r="A2" s="13">
         <v>2018</v>
       </c>
-      <c r="B2" s="15">
-        <v>137.8071</v>
-      </c>
-      <c r="C2" s="15">
-        <v>137.8071</v>
+      <c r="B2" s="13">
+        <v>10.84</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1.33</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="13">
         <v>2019</v>
       </c>
-      <c r="B3" s="15">
-        <v>135.0103</v>
-      </c>
-      <c r="C3" s="15">
-        <v>135.0103</v>
+      <c r="B3" s="13">
+        <v>10.79</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1.71</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:3">
       <c r="A4" s="13">
         <v>2020</v>
       </c>
-      <c r="B4" s="15">
-        <v>130.2591</v>
-      </c>
-      <c r="C4" s="15">
-        <v>130.2591</v>
+      <c r="B4" s="13">
+        <v>10.36</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1.44</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:3">
       <c r="A5" s="13">
         <v>2021</v>
       </c>
-      <c r="B5" s="15">
-        <v>127.3762</v>
-      </c>
-      <c r="C5" s="15">
-        <v>127.3762</v>
+      <c r="B5" s="13">
+        <v>10.01</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1.54</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:3">
       <c r="A6" s="13">
         <v>2022</v>
       </c>
-      <c r="B6" s="15">
-        <v>128.0529</v>
-      </c>
-      <c r="C6" s="15">
-        <v>128.0529</v>
+      <c r="B6" s="13">
+        <v>10.18</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1.18</v>
       </c>
     </row>
     <row r="7" ht="15"/>
@@ -1697,10 +1690,10 @@
   <sheetData>
     <row r="1" ht="58.5" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
@@ -1766,10 +1759,10 @@
   <sheetData>
     <row r="1" ht="44.25" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
@@ -1839,24 +1832,24 @@
   <sheetData>
     <row r="1" ht="15" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6">
         <v>3.6735</v>
@@ -1873,7 +1866,7 @@
     </row>
     <row r="3" ht="15" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="6">
         <v>0.144</v>
@@ -1890,7 +1883,7 @@
     </row>
     <row r="4" ht="15" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="6">
         <v>3.909</v>
@@ -1907,7 +1900,7 @@
     </row>
     <row r="5" ht="15" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6">
         <v>0.7935</v>
@@ -1924,7 +1917,7 @@
     </row>
     <row r="6" ht="15" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="6">
         <v>6.228</v>
@@ -1941,7 +1934,7 @@
     </row>
     <row r="7" ht="15" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="6">
         <v>1.3905</v>
@@ -1958,7 +1951,7 @@
     </row>
     <row r="8" ht="15" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="6">
         <v>0.75</v>
@@ -1975,7 +1968,7 @@
     </row>
     <row r="9" ht="15" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -1988,7 +1981,7 @@
     </row>
     <row r="10" ht="15" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="6">
         <v>0.9195</v>
@@ -2005,7 +1998,7 @@
     </row>
     <row r="11" ht="15" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="6">
         <v>2.0025</v>
@@ -2022,7 +2015,7 @@
     </row>
     <row r="12" ht="15" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="6">
         <v>2.013</v>
@@ -2039,7 +2032,7 @@
     </row>
     <row r="13" ht="15" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6">
@@ -2052,7 +2045,7 @@
     </row>
     <row r="14" ht="15" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6">
@@ -2065,7 +2058,7 @@
     </row>
     <row r="15" ht="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="6">
         <v>1.008</v>
@@ -2082,7 +2075,7 @@
     </row>
     <row r="16" ht="15" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="6">
         <v>0.5595</v>
@@ -2099,7 +2092,7 @@
     </row>
     <row r="17" ht="15" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6">
@@ -2112,7 +2105,7 @@
     </row>
     <row r="18" ht="15" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -2125,7 +2118,7 @@
     </row>
     <row r="19" ht="15" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6">

</xml_diff>

<commit_message>
update hainan aqua chart4
</commit_message>
<xml_diff>
--- a/src/main/resources/data/hainan/水产养殖.xlsx
+++ b/src/main/resources/data/hainan/水产养殖.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="791" activeTab="4"/>
+    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="791" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="左1-近年水产品养殖面积及构成" sheetId="2" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="左3 -近年海水养殖各类面积占比" sheetId="3" r:id="rId3"/>
     <sheet name="右1-近年养殖水产品产量及构成" sheetId="12" r:id="rId4"/>
     <sheet name="右2-近年捕捞水产品产量及构成" sheetId="13" r:id="rId5"/>
-    <sheet name="右3-近年淡水产品产量情况" sheetId="14" r:id="rId6"/>
+    <sheet name="右3-2022年渔业分类产值情况" sheetId="14" r:id="rId6"/>
     <sheet name="中下--2022各品类产量情况" sheetId="11" r:id="rId7"/>
     <sheet name="地图-2022年各市县水产养殖情况（面积、产量）" sheetId="9" r:id="rId8"/>
   </sheets>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>水产品养殖（万亩）</t>
   </si>
@@ -87,11 +87,34 @@
 </t>
   </si>
   <si>
+    <t>各类别产值（万元）</t>
+  </si>
+  <si>
+    <t>海水养殖</t>
+  </si>
+  <si>
+    <t>淡水养殖</t>
+  </si>
+  <si>
+    <t>海水捕捞</t>
+  </si>
+  <si>
+    <t>淡水捕捞</t>
+  </si>
+  <si>
+    <t>水产苗种</t>
+  </si>
+  <si>
+    <t xml:space="preserve">休闲渔业 </t>
+  </si>
+  <si>
+    <t>水产品加工</t>
+  </si>
+  <si>
+    <t>水产流通</t>
+  </si>
+  <si>
     <t>水产养殖</t>
-  </si>
-  <si>
-    <t xml:space="preserve">淡水产品产量(万吨)
-</t>
   </si>
   <si>
     <t xml:space="preserve">2022年产量(万吨)
@@ -1594,7 +1617,7 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
@@ -1677,66 +1700,89 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
   <cols>
-    <col min="2" max="2" width="9" style="1"/>
+    <col min="1" max="1" width="24.125" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="58.5" spans="1:2">
-      <c r="A1" s="11" t="s">
+    <row r="1" ht="39.75" spans="1:2">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="12" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:2">
-      <c r="A2" s="13">
-        <v>2018</v>
-      </c>
-      <c r="B2" s="14">
-        <v>38.0117</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" spans="1:2">
-      <c r="A3" s="13">
-        <v>2019</v>
-      </c>
-      <c r="B3" s="14">
-        <v>37.1468</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" spans="1:2">
-      <c r="A4" s="13">
-        <v>2020</v>
-      </c>
-      <c r="B4" s="14">
-        <v>36.5287</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" spans="1:2">
-      <c r="A5" s="13">
-        <v>2021</v>
-      </c>
-      <c r="B5" s="14">
-        <v>36.7156</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" spans="1:2">
-      <c r="A6" s="13">
-        <v>2022</v>
-      </c>
-      <c r="B6" s="14">
-        <v>42.2581</v>
-      </c>
-    </row>
-    <row r="7" ht="15"/>
+      <c r="B2" s="13">
+        <v>832785.06</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="13">
+        <v>452556.46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="13">
+        <v>3345917.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="13">
+        <v>34852.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="13">
+        <v>353845</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="1:2">
+      <c r="A7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="13">
+        <v>173591</v>
+      </c>
+    </row>
+    <row r="8" ht="27" spans="1:2">
+      <c r="A8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="13">
+        <v>479968.62</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" spans="1:2">
+      <c r="A9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="13">
+        <v>218282.43</v>
+      </c>
+    </row>
+    <row r="10" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1759,10 +1805,10 @@
   <sheetData>
     <row r="1" ht="44.25" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
@@ -1832,24 +1878,24 @@
   <sheetData>
     <row r="1" ht="15" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" ht="15" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B2" s="6">
         <v>3.6735</v>
@@ -1866,7 +1912,7 @@
     </row>
     <row r="3" ht="15" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B3" s="6">
         <v>0.144</v>
@@ -1883,7 +1929,7 @@
     </row>
     <row r="4" ht="15" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6">
         <v>3.909</v>
@@ -1900,7 +1946,7 @@
     </row>
     <row r="5" ht="15" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B5" s="6">
         <v>0.7935</v>
@@ -1917,7 +1963,7 @@
     </row>
     <row r="6" ht="15" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B6" s="6">
         <v>6.228</v>
@@ -1934,7 +1980,7 @@
     </row>
     <row r="7" ht="15" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6">
         <v>1.3905</v>
@@ -1951,7 +1997,7 @@
     </row>
     <row r="8" ht="15" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B8" s="6">
         <v>0.75</v>
@@ -1968,7 +2014,7 @@
     </row>
     <row r="9" ht="15" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -1981,7 +2027,7 @@
     </row>
     <row r="10" ht="15" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6">
         <v>0.9195</v>
@@ -1998,7 +2044,7 @@
     </row>
     <row r="11" ht="15" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B11" s="6">
         <v>2.0025</v>
@@ -2015,7 +2061,7 @@
     </row>
     <row r="12" ht="15" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6">
         <v>2.013</v>
@@ -2032,7 +2078,7 @@
     </row>
     <row r="13" ht="15" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6">
@@ -2045,7 +2091,7 @@
     </row>
     <row r="14" ht="15" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6">
@@ -2058,7 +2104,7 @@
     </row>
     <row r="15" ht="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B15" s="6">
         <v>1.008</v>
@@ -2075,7 +2121,7 @@
     </row>
     <row r="16" ht="15" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B16" s="6">
         <v>0.5595</v>
@@ -2092,7 +2138,7 @@
     </row>
     <row r="17" ht="15" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6">
@@ -2105,7 +2151,7 @@
     </row>
     <row r="18" ht="15" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -2118,7 +2164,7 @@
     </row>
     <row r="19" ht="15" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6">

</xml_diff>